<commit_message>
přidání částí od linkaja1
</commit_message>
<xml_diff>
--- a/Ostatní/Výkaz práce - tým.xlsx
+++ b/Ostatní/Výkaz práce - tým.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="375" windowWidth="18825" windowHeight="7065"/>
+    <workbookView xWindow="312" yWindow="372" windowWidth="18828" windowHeight="7068"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
     <sheet name="List2" sheetId="2" r:id="rId2"/>
     <sheet name="List3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
   <si>
     <t>Beránek Petr</t>
   </si>
@@ -190,13 +191,34 @@
   </si>
   <si>
     <t>Vytvoření use-case – Databáze zvířat</t>
+  </si>
+  <si>
+    <t>Zjištení informací pro implementaci - frameworky</t>
+  </si>
+  <si>
+    <t>SWOT analýza - obecné informace a vytvoření</t>
+  </si>
+  <si>
+    <t>Přidání relevantních informací z ostatních zdrojů do SWOT</t>
+  </si>
+  <si>
+    <t>Obecné požadavky - přepracování</t>
+  </si>
+  <si>
+    <t>GitHub - vytvoření, nastavení, pozvánky</t>
+  </si>
+  <si>
+    <t>GitHub - asistence pro ostatní</t>
+  </si>
+  <si>
+    <t>Tvorba BPM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -878,7 +900,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -891,7 +913,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv sady Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv systému Office">
   <a:themeElements>
     <a:clrScheme name="Kancelář">
       <a:dk1>
@@ -965,6 +987,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -999,6 +1022,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kancelář">
@@ -1174,30 +1198,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="42.6" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="42.6" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.5703125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.5546875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="18"/>
       <c r="B1" s="46" t="s">
         <v>0</v>
@@ -1220,7 +1244,7 @@
       </c>
       <c r="K1" s="38"/>
     </row>
-    <row r="2" spans="1:11" ht="30.75" thickBot="1">
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1255,7 +1279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="42.6" customHeight="1">
+    <row r="3" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="44" t="s">
         <v>8</v>
       </c>
@@ -1271,8 +1295,12 @@
       <c r="E3" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="25"/>
+      <c r="F3" s="24">
+        <v>1</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>58</v>
+      </c>
       <c r="H3" s="12">
         <v>1</v>
       </c>
@@ -1286,7 +1314,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="42.6" customHeight="1">
+    <row r="4" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="42"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -1307,7 +1335,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+    <row r="5" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="45"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
@@ -1324,7 +1352,7 @@
       <c r="J5" s="6"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" ht="42.6" customHeight="1">
+    <row r="6" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="41" t="s">
         <v>22</v>
       </c>
@@ -1340,8 +1368,12 @@
       <c r="E6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
+      <c r="F6" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>59</v>
+      </c>
       <c r="H6" s="16">
         <v>1</v>
       </c>
@@ -1355,7 +1387,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="42.6" customHeight="1">
+    <row r="7" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="42"/>
       <c r="B7" s="4">
         <v>2.5</v>
@@ -1372,7 +1404,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+    <row r="8" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="43"/>
       <c r="B8" s="29">
         <v>0.75</v>
@@ -1389,7 +1421,7 @@
       <c r="J8" s="29"/>
       <c r="K8" s="30"/>
     </row>
-    <row r="9" spans="1:11" ht="42.6" customHeight="1">
+    <row r="9" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="44" t="s">
         <v>21</v>
       </c>
@@ -1405,8 +1437,12 @@
       <c r="E9" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="25"/>
+      <c r="F9" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>60</v>
+      </c>
       <c r="H9" s="12">
         <v>0.5</v>
       </c>
@@ -1420,7 +1456,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="42.6" customHeight="1">
+    <row r="10" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="42"/>
       <c r="B10" s="4">
         <v>3.25</v>
@@ -1441,7 +1477,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="42.6" customHeight="1">
+    <row r="11" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="42"/>
       <c r="B11" s="4">
         <v>2</v>
@@ -1458,7 +1494,7 @@
       <c r="J11" s="4"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+    <row r="12" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="45"/>
       <c r="B12" s="6">
         <v>3</v>
@@ -1475,7 +1511,7 @@
       <c r="J12" s="6"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" ht="42.6" customHeight="1">
+    <row r="13" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="41" t="s">
         <v>20</v>
       </c>
@@ -1491,8 +1527,12 @@
       <c r="E13" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
+      <c r="F13" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>61</v>
+      </c>
       <c r="H13" s="16">
         <v>2</v>
       </c>
@@ -1506,7 +1546,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+    <row r="14" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="43"/>
       <c r="B14" s="29">
         <v>4.5</v>
@@ -1531,7 +1571,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="42.6" customHeight="1">
+    <row r="15" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="44" t="s">
         <v>29</v>
       </c>
@@ -1547,8 +1587,12 @@
       <c r="E15" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="25"/>
+      <c r="F15" s="24">
+        <v>1.5</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>62</v>
+      </c>
       <c r="H15" s="12">
         <v>1.5</v>
       </c>
@@ -1562,7 +1606,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="42.6" customHeight="1">
+    <row r="16" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="42"/>
       <c r="B16" s="4">
         <v>4.5</v>
@@ -1576,8 +1620,12 @@
       <c r="E16" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="5"/>
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="H16" s="10">
         <v>1.5</v>
       </c>
@@ -1591,14 +1639,18 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="42.6" customHeight="1">
+    <row r="17" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="42"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="10"/>
       <c r="E17" s="8"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="5"/>
+      <c r="F17" s="4">
+        <v>6</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="H17" s="10">
         <v>1.5</v>
       </c>
@@ -1612,7 +1664,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="42.6" customHeight="1">
+    <row r="18" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="42"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
@@ -1633,7 +1685,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="42.6" customHeight="1">
+    <row r="19" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="42"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
@@ -1654,7 +1706,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="42.6" customHeight="1">
+    <row r="20" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="42"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
@@ -1671,7 +1723,7 @@
       <c r="J20" s="4"/>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+    <row r="21" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="45"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
@@ -1688,7 +1740,7 @@
       <c r="J21" s="6"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+    <row r="22" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>45</v>
       </c>
@@ -1704,7 +1756,7 @@
       <c r="E22" s="36"/>
       <c r="F22" s="33">
         <f>SUM(F3:F21)</f>
-        <v>0</v>
+        <v>12.25</v>
       </c>
       <c r="G22" s="34"/>
       <c r="H22" s="35">
@@ -1737,24 +1789,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
prerozdeleni bodu a rozsireni vykazu
</commit_message>
<xml_diff>
--- a/Ostatní/Výkaz práce - tým.xlsx
+++ b/Ostatní/Výkaz práce - tým.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="312" yWindow="372" windowWidth="18828" windowHeight="7068"/>
+    <workbookView xWindow="315" yWindow="375" windowWidth="18825" windowHeight="7065"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
     <sheet name="List2" sheetId="2" r:id="rId2"/>
     <sheet name="List3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
   <si>
     <t>Beránek Petr</t>
   </si>
@@ -154,9 +153,6 @@
     <t>Štíbal Petr</t>
   </si>
   <si>
-    <t>Celkem</t>
-  </si>
-  <si>
     <t>Prohledání na internetu, některé projekty tykající se zoologických zahrad a nabídky zoologických zahrad</t>
   </si>
   <si>
@@ -212,6 +208,24 @@
   </si>
   <si>
     <t>Tvorba BPM</t>
+  </si>
+  <si>
+    <t>Oprava diagramů a use-case</t>
+  </si>
+  <si>
+    <t>Tvorba scénářů</t>
+  </si>
+  <si>
+    <t>6.týden</t>
+  </si>
+  <si>
+    <t>Celkem k 1. iteraci</t>
+  </si>
+  <si>
+    <t>7.týden</t>
+  </si>
+  <si>
+    <t>Celkem k 2. iteraci</t>
   </si>
 </sst>
 </file>
@@ -236,7 +250,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -759,11 +773,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -865,38 +938,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1199,52 +1293,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="42.6" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="42.6" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.5546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.5546875" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.5703125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="39" t="s">
+      <c r="C1" s="45"/>
+      <c r="D1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="37" t="s">
+      <c r="E1" s="43"/>
+      <c r="F1" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="39" t="s">
+      <c r="G1" s="47"/>
+      <c r="H1" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="40"/>
-      <c r="J1" s="37" t="s">
+      <c r="I1" s="43"/>
+      <c r="J1" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="38"/>
-    </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K1" s="47"/>
+    </row>
+    <row r="2" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1279,8 +1373,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="44" t="s">
+    <row r="3" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="24">
@@ -1299,7 +1393,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H3" s="12">
         <v>1</v>
@@ -1311,11 +1405,11 @@
         <v>1</v>
       </c>
       <c r="K3" s="25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="42"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="40"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="13"/>
@@ -1332,11 +1426,11 @@
         <v>1.5</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="45"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="41"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
       <c r="D5" s="28"/>
@@ -1352,8 +1446,8 @@
       <c r="J5" s="6"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="41" t="s">
+    <row r="6" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="14">
@@ -1372,7 +1466,7 @@
         <v>1.5</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H6" s="16">
         <v>1</v>
@@ -1384,11 +1478,11 @@
         <v>0.75</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="42"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="40"/>
       <c r="B7" s="4">
         <v>2.5</v>
       </c>
@@ -1404,8 +1498,8 @@
       <c r="J7" s="4"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="43"/>
+    <row r="8" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="38"/>
       <c r="B8" s="29">
         <v>0.75</v>
       </c>
@@ -1421,8 +1515,8 @@
       <c r="J8" s="29"/>
       <c r="K8" s="30"/>
     </row>
-    <row r="9" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="44" t="s">
+    <row r="9" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="39" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="24">
@@ -1441,7 +1535,7 @@
         <v>0.5</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H9" s="12">
         <v>0.5</v>
@@ -1453,11 +1547,11 @@
         <v>0.5</v>
       </c>
       <c r="K9" s="25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="42"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="40"/>
       <c r="B10" s="4">
         <v>3.25</v>
       </c>
@@ -1474,11 +1568,11 @@
         <v>2.5</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="42"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="40"/>
       <c r="B11" s="4">
         <v>2</v>
       </c>
@@ -1494,8 +1588,8 @@
       <c r="J11" s="4"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="45"/>
+    <row r="12" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="41"/>
       <c r="B12" s="6">
         <v>3</v>
       </c>
@@ -1511,8 +1605,8 @@
       <c r="J12" s="6"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="41" t="s">
+    <row r="13" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="37" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="14">
@@ -1531,7 +1625,7 @@
         <v>0.75</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H13" s="16">
         <v>2</v>
@@ -1543,11 +1637,11 @@
         <v>3.25</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="43"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="38"/>
       <c r="B14" s="29">
         <v>4.5</v>
       </c>
@@ -1568,11 +1662,11 @@
         <v>0.5</v>
       </c>
       <c r="K14" s="30" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="39" t="s">
         <v>29</v>
       </c>
       <c r="B15" s="24">
@@ -1591,7 +1685,7 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H15" s="12">
         <v>1.5</v>
@@ -1603,11 +1697,11 @@
         <v>1.5</v>
       </c>
       <c r="K15" s="25" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="42"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="40"/>
       <c r="B16" s="4">
         <v>4.5</v>
       </c>
@@ -1624,7 +1718,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H16" s="10">
         <v>1.5</v>
@@ -1636,11 +1730,11 @@
         <v>1.5</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="42"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="40"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="10"/>
@@ -1649,7 +1743,7 @@
         <v>6</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H17" s="10">
         <v>1.5</v>
@@ -1661,11 +1755,11 @@
         <v>1.5</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="42"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="40"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="10"/>
@@ -1682,11 +1776,11 @@
         <v>1.75</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="42"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="40"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="10"/>
@@ -1703,11 +1797,11 @@
         <v>1.5</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="42"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="40"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="10"/>
@@ -1723,8 +1817,8 @@
       <c r="J20" s="4"/>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="45"/>
+    <row r="21" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="41"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
       <c r="D21" s="11"/>
@@ -1740,20 +1834,20 @@
       <c r="J21" s="6"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B22" s="33">
         <f>SUM(B3:B21)</f>
         <v>26.75</v>
       </c>
       <c r="C22" s="34"/>
-      <c r="D22" s="35">
+      <c r="D22" s="21">
         <f>SUM(D3:D21)</f>
         <v>17.5</v>
       </c>
-      <c r="E22" s="36"/>
+      <c r="E22" s="22"/>
       <c r="F22" s="33">
         <f>SUM(F3:F21)</f>
         <v>12.25</v>
@@ -1770,18 +1864,89 @@
       </c>
       <c r="K22" s="34"/>
     </row>
+    <row r="23" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="51"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="51">
+        <v>2</v>
+      </c>
+      <c r="E23" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="51"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="50"/>
+    </row>
+    <row r="24" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="52"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="52">
+        <v>2</v>
+      </c>
+      <c r="E24" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="52"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="54"/>
+    </row>
+    <row r="25" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="51">
+        <f>SUM(B22:B24)</f>
+        <v>26.75</v>
+      </c>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51">
+        <f t="shared" ref="C25:K25" si="0">SUM(D22:D24)</f>
+        <v>21.5</v>
+      </c>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51">
+        <f t="shared" si="0"/>
+        <v>12.25</v>
+      </c>
+      <c r="G25" s="51"/>
+      <c r="H25" s="51">
+        <f t="shared" si="0"/>
+        <v>19.25</v>
+      </c>
+      <c r="I25" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="51">
+        <f t="shared" si="0"/>
+        <v>17.75</v>
+      </c>
+      <c r="K25" s="51"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A15:A21"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1794,7 +1959,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1806,7 +1971,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>